<commit_message>
SSDM-55: fixed xls exporter to export multivalue property data
</commit_message>
<xml_diff>
--- a/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-omitted-vocabulary-property-compatible-with-import.xlsx
+++ b/server-application-server/sourceTest/java/ch/ethz/sis/openbis/generic/server/xls/export/resources/export-sample-type-with-omitted-vocabulary-property-compatible-with-import.xlsx
@@ -276,7 +276,7 @@
   <dimension ref="A1:L22"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L12" activeCellId="0" sqref="L12:L15"/>
+      <selection pane="topLeft" activeCell="L16" activeCellId="0" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -626,6 +626,8 @@
         <v>22</v>
       </c>
     </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>